<commit_message>
Updates to address #5
</commit_message>
<xml_diff>
--- a/testing/Core7-BiomassHurrane2.0-AK/EvennessWindReductions.xlsx
+++ b/testing/Core7-BiomassHurrane2.0-AK/EvennessWindReductions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rschell\Documents\GitHub\Extension-Base-Hurricane\testing\Core7-BaseHurrane2.0-AK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rschell\Documents\GitHub\Extension-Base-Hurricane\testing\Core7-BiomassHurrane2.0-AK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353DF10C-2DAA-47BF-B3D3-8BADC98F8090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5995D4C-236C-48CE-9575-765925EAC641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CE310B4-5A36-4C79-9D17-85ABE4C06913}"/>
+    <workbookView xWindow="4392" yWindow="1980" windowWidth="23040" windowHeight="13704" xr2:uid="{4CE310B4-5A36-4C79-9D17-85ABE4C06913}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,17 +396,17 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,17 +414,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.5</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>0.25</v>

</xml_diff>